<commit_message>
10.09.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/September/All Details/10.09.2020/MC Bank Statement Sep-2020.xlsx
+++ b/2020/September/All Details/10.09.2020/MC Bank Statement Sep-2020.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="206">
   <si>
     <t>Date</t>
   </si>
@@ -587,9 +587,6 @@
     <t>03.08.2020</t>
   </si>
   <si>
-    <t>Sohag + Mondol</t>
-  </si>
-  <si>
     <t>Mobile bill DSR</t>
   </si>
   <si>
@@ -618,6 +615,36 @@
   </si>
   <si>
     <t>Date: 10.09.2020</t>
+  </si>
+  <si>
+    <t>10.09.2020</t>
+  </si>
+  <si>
+    <t>10.9.2020</t>
+  </si>
+  <si>
+    <t>bKash Jafor</t>
+  </si>
+  <si>
+    <t>BL120</t>
+  </si>
+  <si>
+    <t>Rakib Care CC</t>
+  </si>
+  <si>
+    <t>Z16</t>
+  </si>
+  <si>
+    <t>Mimi Elec Lalpur</t>
+  </si>
+  <si>
+    <t>Fahim Abdulpur0\</t>
+  </si>
+  <si>
+    <t>Dighi Tel</t>
+  </si>
+  <si>
+    <t>`1</t>
   </si>
 </sst>
 </file>
@@ -2888,18 +2915,54 @@
     <xf numFmtId="2" fontId="39" fillId="35" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2910,42 +2973,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3039,7 +3066,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3051,7 +3078,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3074,14 +3101,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3118,7 +3145,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3130,7 +3157,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3153,14 +3180,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3515,8 +3542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D29" sqref="D28:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3720,7 +3747,7 @@
     <row r="13" spans="1:8">
       <c r="A13" s="35"/>
       <c r="B13" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="39">
         <v>0</v>
@@ -3739,7 +3766,7 @@
     <row r="14" spans="1:8">
       <c r="A14" s="35"/>
       <c r="B14" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C14" s="39">
         <v>2000000</v>
@@ -3758,7 +3785,7 @@
     <row r="15" spans="1:8">
       <c r="A15" s="35"/>
       <c r="B15" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" s="39">
         <v>450000</v>
@@ -3777,7 +3804,7 @@
     <row r="16" spans="1:8">
       <c r="A16" s="35"/>
       <c r="B16" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" s="39">
         <v>200000</v>
@@ -3796,7 +3823,7 @@
     <row r="17" spans="1:8">
       <c r="A17" s="35"/>
       <c r="B17" s="40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C17" s="39">
         <v>790000</v>
@@ -3814,12 +3841,18 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="35"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
+      <c r="B18" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="39">
+        <v>850000</v>
+      </c>
+      <c r="D18" s="54">
+        <v>1500000</v>
+      </c>
       <c r="E18" s="41">
         <f>E17+C18-D18</f>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="43"/>
@@ -3832,7 +3865,7 @@
       <c r="D19" s="39"/>
       <c r="E19" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="43"/>
@@ -3845,7 +3878,7 @@
       <c r="D20" s="39"/>
       <c r="E20" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F20" s="33"/>
       <c r="G20" s="43"/>
@@ -3858,7 +3891,7 @@
       <c r="D21" s="39"/>
       <c r="E21" s="41">
         <f>E20+C21-D21</f>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F21" s="31"/>
       <c r="G21" s="2"/>
@@ -3871,7 +3904,7 @@
       <c r="D22" s="39"/>
       <c r="E22" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="2"/>
@@ -3884,7 +3917,7 @@
       <c r="D23" s="39"/>
       <c r="E23" s="41">
         <f>E22+C23-D23</f>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F23" s="31"/>
       <c r="G23" s="2"/>
@@ -3897,7 +3930,7 @@
       <c r="D24" s="39"/>
       <c r="E24" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F24" s="31"/>
       <c r="G24" s="2"/>
@@ -3910,7 +3943,7 @@
       <c r="D25" s="39"/>
       <c r="E25" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F25" s="31"/>
       <c r="G25" s="2"/>
@@ -3923,7 +3956,7 @@
       <c r="D26" s="39"/>
       <c r="E26" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F26" s="31"/>
       <c r="G26" s="2"/>
@@ -3936,7 +3969,7 @@
       <c r="D27" s="39"/>
       <c r="E27" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F27" s="31"/>
       <c r="G27" s="2"/>
@@ -3949,7 +3982,7 @@
       <c r="D28" s="39"/>
       <c r="E28" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F28" s="31"/>
       <c r="G28" s="2"/>
@@ -3962,7 +3995,7 @@
       <c r="D29" s="39"/>
       <c r="E29" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F29" s="31"/>
       <c r="G29" s="2"/>
@@ -3975,7 +4008,7 @@
       <c r="D30" s="39"/>
       <c r="E30" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F30" s="31"/>
       <c r="G30" s="2"/>
@@ -3988,7 +4021,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F31" s="31"/>
       <c r="G31" s="2"/>
@@ -4001,7 +4034,7 @@
       <c r="D32" s="39"/>
       <c r="E32" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F32" s="31"/>
       <c r="G32" s="2"/>
@@ -4014,7 +4047,7 @@
       <c r="D33" s="42"/>
       <c r="E33" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F33" s="31"/>
       <c r="G33" s="2"/>
@@ -4027,7 +4060,7 @@
       <c r="D34" s="39"/>
       <c r="E34" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F34" s="31"/>
       <c r="G34" s="2"/>
@@ -4040,7 +4073,7 @@
       <c r="D35" s="39"/>
       <c r="E35" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F35" s="31"/>
       <c r="G35" s="2"/>
@@ -4053,7 +4086,7 @@
       <c r="D36" s="39"/>
       <c r="E36" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F36" s="31"/>
       <c r="G36" s="2"/>
@@ -4066,7 +4099,7 @@
       <c r="D37" s="39"/>
       <c r="E37" s="41">
         <f t="shared" si="0"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F37" s="31"/>
       <c r="G37" s="2"/>
@@ -4079,7 +4112,7 @@
       <c r="D38" s="39"/>
       <c r="E38" s="41">
         <f t="shared" ref="E38:E69" si="1">E37+C38-D38</f>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F38" s="31"/>
       <c r="G38" s="2"/>
@@ -4092,7 +4125,7 @@
       <c r="D39" s="39"/>
       <c r="E39" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F39" s="31"/>
       <c r="G39" s="2"/>
@@ -4105,7 +4138,7 @@
       <c r="D40" s="39"/>
       <c r="E40" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F40" s="31"/>
       <c r="G40" s="2"/>
@@ -4118,7 +4151,7 @@
       <c r="D41" s="39"/>
       <c r="E41" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F41" s="31"/>
       <c r="G41" s="2"/>
@@ -4131,7 +4164,7 @@
       <c r="D42" s="39"/>
       <c r="E42" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F42" s="31"/>
       <c r="G42" s="2"/>
@@ -4144,7 +4177,7 @@
       <c r="D43" s="39"/>
       <c r="E43" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F43" s="31"/>
       <c r="G43" s="2"/>
@@ -4157,7 +4190,7 @@
       <c r="D44" s="39"/>
       <c r="E44" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F44" s="31"/>
       <c r="G44" s="2"/>
@@ -4170,7 +4203,7 @@
       <c r="D45" s="39"/>
       <c r="E45" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F45" s="31"/>
       <c r="G45" s="2"/>
@@ -4183,7 +4216,7 @@
       <c r="D46" s="39"/>
       <c r="E46" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F46" s="31"/>
       <c r="G46" s="2"/>
@@ -4196,7 +4229,7 @@
       <c r="D47" s="39"/>
       <c r="E47" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F47" s="31"/>
       <c r="G47" s="2"/>
@@ -4209,7 +4242,7 @@
       <c r="D48" s="39"/>
       <c r="E48" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F48" s="31"/>
       <c r="G48" s="2"/>
@@ -4221,7 +4254,7 @@
       <c r="D49" s="39"/>
       <c r="E49" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F49" s="31"/>
       <c r="G49" s="2"/>
@@ -4233,7 +4266,7 @@
       <c r="D50" s="39"/>
       <c r="E50" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F50" s="31"/>
       <c r="G50" s="2"/>
@@ -4245,7 +4278,7 @@
       <c r="D51" s="39"/>
       <c r="E51" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F51" s="31"/>
       <c r="G51" s="2"/>
@@ -4257,7 +4290,7 @@
       <c r="D52" s="39"/>
       <c r="E52" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F52" s="31"/>
       <c r="G52" s="2"/>
@@ -4269,7 +4302,7 @@
       <c r="D53" s="39"/>
       <c r="E53" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F53" s="31"/>
       <c r="G53" s="2"/>
@@ -4281,7 +4314,7 @@
       <c r="D54" s="39"/>
       <c r="E54" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F54" s="31"/>
       <c r="G54" s="2"/>
@@ -4293,7 +4326,7 @@
       <c r="D55" s="39"/>
       <c r="E55" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F55" s="31"/>
       <c r="G55" s="2"/>
@@ -4304,7 +4337,7 @@
       <c r="D56" s="39"/>
       <c r="E56" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F56" s="31"/>
       <c r="G56" s="2"/>
@@ -4315,7 +4348,7 @@
       <c r="D57" s="39"/>
       <c r="E57" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F57" s="31"/>
       <c r="G57" s="2"/>
@@ -4326,7 +4359,7 @@
       <c r="D58" s="39"/>
       <c r="E58" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F58" s="31"/>
       <c r="G58" s="2"/>
@@ -4337,7 +4370,7 @@
       <c r="D59" s="39"/>
       <c r="E59" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F59" s="31"/>
       <c r="G59" s="2"/>
@@ -4348,7 +4381,7 @@
       <c r="D60" s="39"/>
       <c r="E60" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F60" s="31"/>
       <c r="G60" s="2"/>
@@ -4359,7 +4392,7 @@
       <c r="D61" s="39"/>
       <c r="E61" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F61" s="31"/>
       <c r="G61" s="2"/>
@@ -4370,7 +4403,7 @@
       <c r="D62" s="39"/>
       <c r="E62" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F62" s="31"/>
       <c r="G62" s="2"/>
@@ -4381,7 +4414,7 @@
       <c r="D63" s="39"/>
       <c r="E63" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F63" s="31"/>
       <c r="G63" s="2"/>
@@ -4392,7 +4425,7 @@
       <c r="D64" s="39"/>
       <c r="E64" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F64" s="31"/>
       <c r="G64" s="2"/>
@@ -4403,7 +4436,7 @@
       <c r="D65" s="39"/>
       <c r="E65" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F65" s="31"/>
       <c r="G65" s="2"/>
@@ -4414,7 +4447,7 @@
       <c r="D66" s="39"/>
       <c r="E66" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F66" s="31"/>
       <c r="G66" s="2"/>
@@ -4425,7 +4458,7 @@
       <c r="D67" s="39"/>
       <c r="E67" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F67" s="31"/>
       <c r="G67" s="2"/>
@@ -4436,7 +4469,7 @@
       <c r="D68" s="39"/>
       <c r="E68" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F68" s="31"/>
       <c r="G68" s="2"/>
@@ -4447,7 +4480,7 @@
       <c r="D69" s="39"/>
       <c r="E69" s="41">
         <f t="shared" si="1"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F69" s="31"/>
       <c r="G69" s="2"/>
@@ -4458,7 +4491,7 @@
       <c r="D70" s="39"/>
       <c r="E70" s="41">
         <f t="shared" ref="E70:E82" si="2">E69+C70-D70</f>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F70" s="31"/>
       <c r="G70" s="2"/>
@@ -4469,7 +4502,7 @@
       <c r="D71" s="39"/>
       <c r="E71" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F71" s="31"/>
       <c r="G71" s="2"/>
@@ -4480,7 +4513,7 @@
       <c r="D72" s="39"/>
       <c r="E72" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F72" s="31"/>
       <c r="G72" s="2"/>
@@ -4491,7 +4524,7 @@
       <c r="D73" s="39"/>
       <c r="E73" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F73" s="31"/>
       <c r="G73" s="2"/>
@@ -4502,7 +4535,7 @@
       <c r="D74" s="39"/>
       <c r="E74" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F74" s="31"/>
       <c r="G74" s="2"/>
@@ -4513,7 +4546,7 @@
       <c r="D75" s="39"/>
       <c r="E75" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F75" s="33"/>
       <c r="G75" s="2"/>
@@ -4524,7 +4557,7 @@
       <c r="D76" s="39"/>
       <c r="E76" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F76" s="31"/>
       <c r="G76" s="2"/>
@@ -4535,7 +4568,7 @@
       <c r="D77" s="39"/>
       <c r="E77" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F77" s="31"/>
       <c r="G77" s="2"/>
@@ -4546,7 +4579,7 @@
       <c r="D78" s="39"/>
       <c r="E78" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F78" s="31"/>
       <c r="G78" s="2"/>
@@ -4557,7 +4590,7 @@
       <c r="D79" s="39"/>
       <c r="E79" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F79" s="31"/>
       <c r="G79" s="2"/>
@@ -4568,7 +4601,7 @@
       <c r="D80" s="39"/>
       <c r="E80" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F80" s="31"/>
       <c r="G80" s="2"/>
@@ -4579,7 +4612,7 @@
       <c r="D81" s="39"/>
       <c r="E81" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F81" s="31"/>
       <c r="G81" s="2"/>
@@ -4590,7 +4623,7 @@
       <c r="D82" s="39"/>
       <c r="E82" s="41">
         <f t="shared" si="2"/>
-        <v>2845874</v>
+        <v>2195874</v>
       </c>
       <c r="F82" s="31"/>
       <c r="G82" s="2"/>
@@ -4599,15 +4632,15 @@
       <c r="B83" s="45"/>
       <c r="C83" s="41">
         <f>SUM(C5:C72)</f>
-        <v>8645874</v>
+        <v>9495874</v>
       </c>
       <c r="D83" s="41">
         <f>SUM(D5:D77)</f>
-        <v>5800000</v>
+        <v>7300000</v>
       </c>
       <c r="E83" s="67">
         <f>E71+C83-D83</f>
-        <v>5691748</v>
+        <v>4391748</v>
       </c>
       <c r="F83" s="32"/>
       <c r="G83" s="2"/>
@@ -4636,7 +4669,7 @@
   <dimension ref="A1:AC222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" customHeight="1"/>
@@ -4664,7 +4697,7 @@
     </row>
     <row r="2" spans="1:29" ht="23.25">
       <c r="A2" s="305" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="306"/>
       <c r="C2" s="306"/>
@@ -4777,7 +4810,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="73">
-        <v>0</v>
+        <v>2195874</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="56"/>
@@ -4817,7 +4850,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="74">
-        <v>0</v>
+        <v>1072892</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="56"/>
@@ -4854,7 +4887,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="75">
-        <v>0</v>
+        <v>2273533</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="56"/>
@@ -4886,7 +4919,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="72">
-        <v>0</v>
+        <v>21913</v>
       </c>
       <c r="C8" s="71"/>
       <c r="D8" s="69" t="s">
@@ -4965,14 +4998,14 @@
       </c>
       <c r="B10" s="77">
         <f>B5-B8-B9</f>
-        <v>172797.44500000001</v>
+        <v>150884.44500000001</v>
       </c>
       <c r="C10" s="71"/>
       <c r="D10" s="69" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="75">
-        <v>0</v>
+        <v>1801624.9850000003</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="50"/>
@@ -5004,7 +5037,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="76">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="C11" s="71"/>
       <c r="D11" s="71"/>
@@ -5075,7 +5108,7 @@
       </c>
       <c r="B13" s="76">
         <f>B6-B8-B11+B12-B9</f>
-        <v>8673165.4450000003</v>
+        <v>8621252.4450000003</v>
       </c>
       <c r="C13" s="71"/>
       <c r="D13" s="71" t="s">
@@ -5083,12 +5116,12 @@
       </c>
       <c r="E13" s="75">
         <f>E4+E5+E6+E7+E8+E9+E10</f>
-        <v>1277328.46</v>
+        <v>8621252.4450000003</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="85">
         <f>B13-E13</f>
-        <v>7395836.9850000003</v>
+        <v>0</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="8"/>
@@ -5234,7 +5267,9 @@
       </c>
       <c r="G17" s="30"/>
       <c r="H17" s="28"/>
-      <c r="I17" s="8"/>
+      <c r="I17" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -5306,7 +5341,7 @@
         <v>26</v>
       </c>
       <c r="E19" s="104">
-        <v>54450</v>
+        <v>64450</v>
       </c>
       <c r="G19" s="57"/>
       <c r="H19" s="8"/>
@@ -5344,7 +5379,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="104">
-        <v>154630</v>
+        <v>185000</v>
       </c>
       <c r="G20" s="29"/>
       <c r="H20" s="8"/>
@@ -5375,7 +5410,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="53">
-        <v>379960</v>
+        <v>398960</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="19" t="s">
@@ -10341,7 +10376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A111" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
@@ -10852,7 +10887,7 @@
     </row>
     <row r="8" spans="1:61" ht="12.6" customHeight="1">
       <c r="A8" s="120" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="121">
         <v>850210</v>
@@ -10928,7 +10963,7 @@
     </row>
     <row r="9" spans="1:61" ht="12" customHeight="1">
       <c r="A9" s="120" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" s="121">
         <v>382520</v>
@@ -11004,7 +11039,7 @@
     </row>
     <row r="10" spans="1:61" ht="12.6" customHeight="1">
       <c r="A10" s="120" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="121">
         <v>240040</v>
@@ -11028,7 +11063,7 @@
         <v>705</v>
       </c>
       <c r="J10" s="119" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K10" s="111"/>
       <c r="L10" s="131"/>
@@ -11084,7 +11119,7 @@
     </row>
     <row r="11" spans="1:61" ht="12.6" customHeight="1">
       <c r="A11" s="120" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11" s="121">
         <v>808630</v>
@@ -11108,7 +11143,7 @@
         <v>7525</v>
       </c>
       <c r="J11" s="119" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K11" s="111"/>
       <c r="L11" s="133"/>
@@ -11164,7 +11199,7 @@
     </row>
     <row r="12" spans="1:61" ht="12.6" customHeight="1">
       <c r="A12" s="120" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="121">
         <v>986900</v>
@@ -11188,7 +11223,7 @@
         <v>7345</v>
       </c>
       <c r="J12" s="119" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K12" s="111"/>
       <c r="L12" s="110"/>
@@ -11243,13 +11278,21 @@
       <c r="BI12" s="111"/>
     </row>
     <row r="13" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A13" s="120"/>
-      <c r="B13" s="121"/>
-      <c r="C13" s="121"/>
-      <c r="D13" s="121"/>
+      <c r="A13" s="120" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="121">
+        <v>1155210</v>
+      </c>
+      <c r="C13" s="121">
+        <v>1106422</v>
+      </c>
+      <c r="D13" s="121">
+        <v>3123</v>
+      </c>
       <c r="E13" s="121">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1109545</v>
       </c>
       <c r="F13" s="132"/>
       <c r="G13" s="110"/>
@@ -12612,23 +12655,23 @@
       </c>
       <c r="B33" s="121">
         <f>SUM(B5:B32)</f>
-        <v>5837070</v>
+        <v>6992280</v>
       </c>
       <c r="C33" s="121">
         <f>SUM(C5:C32)</f>
-        <v>5646750</v>
+        <v>6753172</v>
       </c>
       <c r="D33" s="121">
         <f>SUM(D5:D32)</f>
-        <v>18790</v>
+        <v>21913</v>
       </c>
       <c r="E33" s="121">
         <f>SUM(E5:E32)</f>
-        <v>5665540</v>
+        <v>6775085</v>
       </c>
       <c r="F33" s="129">
         <f>B33-E33</f>
-        <v>171530</v>
+        <v>217195</v>
       </c>
       <c r="G33" s="143"/>
       <c r="H33" s="151" t="s">
@@ -13117,7 +13160,7 @@
         <v>8800</v>
       </c>
       <c r="D40" s="161" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E40" s="126"/>
       <c r="F40" s="122"/>
@@ -13188,7 +13231,7 @@
         <v>4100</v>
       </c>
       <c r="D41" s="114" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E41" s="165"/>
       <c r="F41" s="122"/>
@@ -13320,14 +13363,14 @@
     </row>
     <row r="43" spans="1:61" ht="12.6" customHeight="1">
       <c r="A43" s="299" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B43" s="114"/>
       <c r="C43" s="121">
         <v>9300</v>
       </c>
       <c r="D43" s="114" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E43" s="127"/>
       <c r="F43" s="323" t="s">
@@ -13660,7 +13703,7 @@
         <v>218875</v>
       </c>
       <c r="D48" s="188" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E48" s="126"/>
       <c r="F48" s="150"/>
@@ -13861,10 +13904,10 @@
       </c>
       <c r="B51" s="118"/>
       <c r="C51" s="190">
-        <v>62510</v>
+        <v>64440</v>
       </c>
       <c r="D51" s="194" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E51" s="126"/>
       <c r="F51" s="118"/>
@@ -13930,10 +13973,10 @@
       </c>
       <c r="B52" s="191"/>
       <c r="C52" s="196">
-        <v>195000</v>
+        <v>185000</v>
       </c>
       <c r="D52" s="186" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E52" s="126"/>
       <c r="F52" s="150"/>
@@ -13999,10 +14042,10 @@
       </c>
       <c r="B53" s="118"/>
       <c r="C53" s="190">
-        <v>392440</v>
+        <v>398480</v>
       </c>
       <c r="D53" s="197" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E53" s="126"/>
       <c r="F53" s="119"/>
@@ -14068,10 +14111,10 @@
       </c>
       <c r="B54" s="118"/>
       <c r="C54" s="190">
-        <v>190785</v>
+        <v>190485</v>
       </c>
       <c r="D54" s="186" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E54" s="126"/>
       <c r="F54" s="150"/>
@@ -14133,14 +14176,14 @@
     </row>
     <row r="55" spans="1:61" ht="12" customHeight="1">
       <c r="A55" s="195" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="B55" s="191"/>
       <c r="C55" s="190">
-        <v>3730</v>
+        <v>20000</v>
       </c>
       <c r="D55" s="197" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E55" s="126"/>
       <c r="F55" s="118"/>
@@ -14202,14 +14245,14 @@
     </row>
     <row r="56" spans="1:61" ht="12" customHeight="1">
       <c r="A56" s="193" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B56" s="118"/>
       <c r="C56" s="190">
-        <v>18600</v>
+        <v>13740</v>
       </c>
       <c r="D56" s="194" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E56" s="126"/>
       <c r="F56" s="118"/>
@@ -15746,7 +15789,7 @@
         <v>24000</v>
       </c>
       <c r="D76" s="194" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E76" s="126"/>
       <c r="F76" s="209"/>
@@ -16792,7 +16835,7 @@
         <v>28610</v>
       </c>
       <c r="D89" s="194" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E89" s="126"/>
       <c r="F89" s="209"/>
@@ -17024,10 +17067,16 @@
       <c r="BI91" s="111"/>
     </row>
     <row r="92" spans="1:61">
-      <c r="A92" s="193"/>
+      <c r="A92" s="193" t="s">
+        <v>202</v>
+      </c>
       <c r="B92" s="191"/>
-      <c r="C92" s="190"/>
-      <c r="D92" s="191"/>
+      <c r="C92" s="190">
+        <v>24025</v>
+      </c>
+      <c r="D92" s="191" t="s">
+        <v>196</v>
+      </c>
       <c r="F92" s="209"/>
       <c r="G92" s="203" t="s">
         <v>85</v>
@@ -17097,10 +17146,16 @@
       <c r="BI92" s="111"/>
     </row>
     <row r="93" spans="1:61" ht="14.25" customHeight="1">
-      <c r="A93" s="193"/>
+      <c r="A93" s="193" t="s">
+        <v>203</v>
+      </c>
       <c r="B93" s="191"/>
-      <c r="C93" s="190"/>
-      <c r="D93" s="191"/>
+      <c r="C93" s="190">
+        <v>2930</v>
+      </c>
+      <c r="D93" s="191" t="s">
+        <v>196</v>
+      </c>
       <c r="F93" s="209"/>
       <c r="G93" s="203" t="s">
         <v>86</v>
@@ -17391,10 +17446,18 @@
       <c r="BI96" s="111"/>
     </row>
     <row r="97" spans="1:61">
-      <c r="A97" s="193"/>
-      <c r="B97" s="191"/>
-      <c r="C97" s="190"/>
-      <c r="D97" s="191"/>
+      <c r="A97" s="193" t="s">
+        <v>200</v>
+      </c>
+      <c r="B97" s="191" t="s">
+        <v>201</v>
+      </c>
+      <c r="C97" s="190">
+        <v>7790</v>
+      </c>
+      <c r="D97" s="191" t="s">
+        <v>196</v>
+      </c>
       <c r="F97" s="213"/>
       <c r="G97" s="207" t="s">
         <v>100</v>
@@ -17464,10 +17527,18 @@
       <c r="BI97" s="111"/>
     </row>
     <row r="98" spans="1:61">
-      <c r="A98" s="216"/>
-      <c r="B98" s="217"/>
-      <c r="C98" s="190"/>
-      <c r="D98" s="191"/>
+      <c r="A98" s="216" t="s">
+        <v>198</v>
+      </c>
+      <c r="B98" s="217" t="s">
+        <v>199</v>
+      </c>
+      <c r="C98" s="190">
+        <v>1840</v>
+      </c>
+      <c r="D98" s="191" t="s">
+        <v>196</v>
+      </c>
       <c r="F98" s="213"/>
       <c r="G98" s="207" t="s">
         <v>103</v>
@@ -17535,7 +17606,7 @@
     </row>
     <row r="99" spans="1:61">
       <c r="A99" s="216" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B99" s="298">
         <v>44075</v>
@@ -17544,7 +17615,7 @@
         <v>1800</v>
       </c>
       <c r="D99" s="191" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F99" s="213"/>
       <c r="G99" s="207" t="s">
@@ -17845,7 +17916,7 @@
     </row>
     <row r="103" spans="1:61">
       <c r="A103" s="216" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B103" s="217"/>
       <c r="C103" s="190">
@@ -18620,7 +18691,7 @@
       <c r="B113" s="313"/>
       <c r="C113" s="218">
         <f>SUM(C37:C112)</f>
-        <v>2227868</v>
+        <v>2273533</v>
       </c>
       <c r="D113" s="219"/>
       <c r="F113" s="209"/>
@@ -18771,7 +18842,7 @@
       <c r="B115" s="315"/>
       <c r="C115" s="223">
         <f>C113+L136</f>
-        <v>2227868</v>
+        <v>2273533</v>
       </c>
       <c r="D115" s="224"/>
       <c r="F115" s="202"/>
@@ -21390,8 +21461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z321"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21402,94 +21473,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="336" t="s">
+      <c r="A1" s="328" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="336"/>
-      <c r="C1" s="336"/>
-      <c r="D1" s="336"/>
-      <c r="E1" s="336"/>
-      <c r="F1" s="336"/>
-      <c r="G1" s="336"/>
-      <c r="H1" s="336"/>
-      <c r="I1" s="336"/>
-      <c r="J1" s="336"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="336"/>
-      <c r="M1" s="336"/>
-      <c r="N1" s="336"/>
-      <c r="O1" s="336"/>
-      <c r="P1" s="336"/>
-      <c r="Q1" s="336"/>
-      <c r="R1" s="336"/>
-      <c r="S1" s="336"/>
+      <c r="B1" s="328"/>
+      <c r="C1" s="328"/>
+      <c r="D1" s="328"/>
+      <c r="E1" s="328"/>
+      <c r="F1" s="328"/>
+      <c r="G1" s="328"/>
+      <c r="H1" s="328"/>
+      <c r="I1" s="328"/>
+      <c r="J1" s="328"/>
+      <c r="K1" s="328"/>
+      <c r="L1" s="328"/>
+      <c r="M1" s="328"/>
+      <c r="N1" s="328"/>
+      <c r="O1" s="328"/>
+      <c r="P1" s="328"/>
+      <c r="Q1" s="328"/>
+      <c r="R1" s="328"/>
+      <c r="S1" s="328"/>
     </row>
     <row r="2" spans="1:26" s="245" customFormat="1" ht="18">
-      <c r="A2" s="337" t="s">
+      <c r="A2" s="329" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="337"/>
-      <c r="C2" s="337"/>
-      <c r="D2" s="337"/>
-      <c r="E2" s="337"/>
-      <c r="F2" s="337"/>
-      <c r="G2" s="337"/>
-      <c r="H2" s="337"/>
-      <c r="I2" s="337"/>
-      <c r="J2" s="337"/>
-      <c r="K2" s="337"/>
-      <c r="L2" s="337"/>
-      <c r="M2" s="337"/>
-      <c r="N2" s="337"/>
-      <c r="O2" s="337"/>
-      <c r="P2" s="337"/>
-      <c r="Q2" s="337"/>
-      <c r="R2" s="337"/>
-      <c r="S2" s="337"/>
+      <c r="B2" s="329"/>
+      <c r="C2" s="329"/>
+      <c r="D2" s="329"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="329"/>
+      <c r="I2" s="329"/>
+      <c r="J2" s="329"/>
+      <c r="K2" s="329"/>
+      <c r="L2" s="329"/>
+      <c r="M2" s="329"/>
+      <c r="N2" s="329"/>
+      <c r="O2" s="329"/>
+      <c r="P2" s="329"/>
+      <c r="Q2" s="329"/>
+      <c r="R2" s="329"/>
+      <c r="S2" s="329"/>
     </row>
     <row r="3" spans="1:26" s="245" customFormat="1">
-      <c r="A3" s="338"/>
-      <c r="B3" s="338"/>
-      <c r="C3" s="338"/>
-      <c r="D3" s="338"/>
-      <c r="E3" s="338"/>
-      <c r="F3" s="338"/>
-      <c r="G3" s="338"/>
-      <c r="H3" s="338"/>
-      <c r="I3" s="338"/>
-      <c r="J3" s="338"/>
-      <c r="K3" s="338"/>
-      <c r="L3" s="338"/>
-      <c r="M3" s="338"/>
-      <c r="N3" s="338"/>
-      <c r="O3" s="338"/>
-      <c r="P3" s="338"/>
-      <c r="Q3" s="338"/>
-      <c r="R3" s="338"/>
-      <c r="S3" s="338"/>
+      <c r="A3" s="330"/>
+      <c r="B3" s="330"/>
+      <c r="C3" s="330"/>
+      <c r="D3" s="330"/>
+      <c r="E3" s="330"/>
+      <c r="F3" s="330"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="330"/>
+      <c r="J3" s="330"/>
+      <c r="K3" s="330"/>
+      <c r="L3" s="330"/>
+      <c r="M3" s="330"/>
+      <c r="N3" s="330"/>
+      <c r="O3" s="330"/>
+      <c r="P3" s="330"/>
+      <c r="Q3" s="330"/>
+      <c r="R3" s="330"/>
+      <c r="S3" s="330"/>
     </row>
     <row r="4" spans="1:26" s="246" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="339" t="s">
+      <c r="A4" s="331" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="340"/>
-      <c r="C4" s="340"/>
-      <c r="D4" s="340"/>
-      <c r="E4" s="340"/>
-      <c r="F4" s="340"/>
-      <c r="G4" s="340"/>
-      <c r="H4" s="340"/>
-      <c r="I4" s="340"/>
-      <c r="J4" s="340"/>
-      <c r="K4" s="340"/>
-      <c r="L4" s="340"/>
-      <c r="M4" s="340"/>
-      <c r="N4" s="340"/>
-      <c r="O4" s="340"/>
-      <c r="P4" s="340"/>
-      <c r="Q4" s="340"/>
-      <c r="R4" s="340"/>
-      <c r="S4" s="341"/>
+      <c r="B4" s="332"/>
+      <c r="C4" s="332"/>
+      <c r="D4" s="332"/>
+      <c r="E4" s="332"/>
+      <c r="F4" s="332"/>
+      <c r="G4" s="332"/>
+      <c r="H4" s="332"/>
+      <c r="I4" s="332"/>
+      <c r="J4" s="332"/>
+      <c r="K4" s="332"/>
+      <c r="L4" s="332"/>
+      <c r="M4" s="332"/>
+      <c r="N4" s="332"/>
+      <c r="O4" s="332"/>
+      <c r="P4" s="332"/>
+      <c r="Q4" s="332"/>
+      <c r="R4" s="332"/>
+      <c r="S4" s="333"/>
       <c r="U4" s="127"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
@@ -21498,58 +21569,58 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="1:26" s="248" customFormat="1">
-      <c r="A5" s="342" t="s">
+      <c r="A5" s="334" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="344" t="s">
+      <c r="B5" s="336" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="330" t="s">
+      <c r="C5" s="338" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="330" t="s">
+      <c r="D5" s="338" t="s">
         <v>166</v>
       </c>
-      <c r="E5" s="330" t="s">
+      <c r="E5" s="338" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="330" t="s">
+      <c r="F5" s="338" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="330" t="s">
+      <c r="G5" s="338" t="s">
         <v>169</v>
       </c>
-      <c r="H5" s="330" t="s">
+      <c r="H5" s="338" t="s">
         <v>170</v>
       </c>
-      <c r="I5" s="330" t="s">
+      <c r="I5" s="338" t="s">
         <v>171</v>
       </c>
-      <c r="J5" s="330" t="s">
+      <c r="J5" s="338" t="s">
         <v>172</v>
       </c>
-      <c r="K5" s="330" t="s">
+      <c r="K5" s="338" t="s">
         <v>173</v>
       </c>
-      <c r="L5" s="330" t="s">
+      <c r="L5" s="338" t="s">
         <v>174</v>
       </c>
-      <c r="M5" s="330" t="s">
+      <c r="M5" s="338" t="s">
         <v>175</v>
       </c>
-      <c r="N5" s="330" t="s">
+      <c r="N5" s="338" t="s">
         <v>176</v>
       </c>
-      <c r="O5" s="332" t="s">
+      <c r="O5" s="344" t="s">
         <v>177</v>
       </c>
-      <c r="P5" s="334" t="s">
+      <c r="P5" s="346" t="s">
         <v>178</v>
       </c>
-      <c r="Q5" s="328" t="s">
+      <c r="Q5" s="342" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="346" t="s">
+      <c r="R5" s="340" t="s">
         <v>179</v>
       </c>
       <c r="S5" s="247" t="s">
@@ -21562,24 +21633,24 @@
       <c r="Y5" s="250"/>
     </row>
     <row r="6" spans="1:26" s="248" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="343"/>
-      <c r="B6" s="345"/>
-      <c r="C6" s="331"/>
-      <c r="D6" s="331"/>
-      <c r="E6" s="331"/>
-      <c r="F6" s="331"/>
-      <c r="G6" s="331"/>
-      <c r="H6" s="331"/>
-      <c r="I6" s="331"/>
-      <c r="J6" s="331"/>
-      <c r="K6" s="331"/>
-      <c r="L6" s="331"/>
-      <c r="M6" s="331"/>
-      <c r="N6" s="331"/>
-      <c r="O6" s="333"/>
-      <c r="P6" s="335"/>
-      <c r="Q6" s="329"/>
-      <c r="R6" s="347"/>
+      <c r="A6" s="335"/>
+      <c r="B6" s="337"/>
+      <c r="C6" s="339"/>
+      <c r="D6" s="339"/>
+      <c r="E6" s="339"/>
+      <c r="F6" s="339"/>
+      <c r="G6" s="339"/>
+      <c r="H6" s="339"/>
+      <c r="I6" s="339"/>
+      <c r="J6" s="339"/>
+      <c r="K6" s="339"/>
+      <c r="L6" s="339"/>
+      <c r="M6" s="339"/>
+      <c r="N6" s="339"/>
+      <c r="O6" s="345"/>
+      <c r="P6" s="347"/>
+      <c r="Q6" s="343"/>
+      <c r="R6" s="341"/>
       <c r="S6" s="252" t="s">
         <v>180</v>
       </c>
@@ -21726,7 +21797,7 @@
     </row>
     <row r="10" spans="1:26" s="22" customFormat="1">
       <c r="A10" s="256" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="264">
         <v>800</v>
@@ -21768,7 +21839,7 @@
     </row>
     <row r="11" spans="1:26" s="22" customFormat="1">
       <c r="A11" s="256" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="264">
         <v>500</v>
@@ -21810,7 +21881,7 @@
     </row>
     <row r="12" spans="1:26" s="22" customFormat="1">
       <c r="A12" s="256" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="264">
         <v>500</v>
@@ -21852,7 +21923,7 @@
     </row>
     <row r="13" spans="1:26" s="22" customFormat="1">
       <c r="A13" s="256" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="264">
         <v>500</v>
@@ -21898,7 +21969,7 @@
     </row>
     <row r="14" spans="1:26" s="22" customFormat="1">
       <c r="A14" s="256" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14" s="264">
         <v>600</v>
@@ -21941,27 +22012,43 @@
       <c r="Y14" s="48"/>
     </row>
     <row r="15" spans="1:26" s="22" customFormat="1">
-      <c r="A15" s="256"/>
-      <c r="B15" s="264"/>
+      <c r="A15" s="256" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="264">
+        <v>1200</v>
+      </c>
       <c r="C15" s="257"/>
-      <c r="D15" s="265"/>
+      <c r="D15" s="265">
+        <v>98</v>
+      </c>
       <c r="E15" s="265"/>
-      <c r="F15" s="265"/>
-      <c r="G15" s="265"/>
+      <c r="F15" s="265">
+        <v>975</v>
+      </c>
+      <c r="G15" s="265">
+        <v>210</v>
+      </c>
       <c r="H15" s="265"/>
       <c r="I15" s="265"/>
-      <c r="J15" s="265"/>
-      <c r="K15" s="265"/>
+      <c r="J15" s="265">
+        <v>20</v>
+      </c>
+      <c r="K15" s="265">
+        <v>560</v>
+      </c>
       <c r="L15" s="269"/>
       <c r="M15" s="265"/>
-      <c r="N15" s="265"/>
+      <c r="N15" s="265">
+        <v>60</v>
+      </c>
       <c r="O15" s="265"/>
       <c r="P15" s="265"/>
       <c r="Q15" s="265"/>
       <c r="R15" s="267"/>
       <c r="S15" s="261">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3123</v>
       </c>
       <c r="T15" s="262"/>
       <c r="U15" s="270"/>
@@ -22575,7 +22662,7 @@
       </c>
       <c r="B38" s="282">
         <f>SUM(B7:B37)</f>
-        <v>5100</v>
+        <v>6300</v>
       </c>
       <c r="C38" s="283">
         <f t="shared" ref="C38:R38" si="1">SUM(C7:C37)</f>
@@ -22583,7 +22670,7 @@
       </c>
       <c r="D38" s="283">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>228</v>
       </c>
       <c r="E38" s="283">
         <f t="shared" si="1"/>
@@ -22591,7 +22678,7 @@
       </c>
       <c r="F38" s="283">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>975</v>
       </c>
       <c r="G38" s="283"/>
       <c r="H38" s="283">
@@ -22604,11 +22691,11 @@
       </c>
       <c r="J38" s="283">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="K38" s="283">
         <f t="shared" si="1"/>
-        <v>3200</v>
+        <v>3760</v>
       </c>
       <c r="L38" s="283">
         <f t="shared" si="1"/>
@@ -22620,7 +22707,7 @@
       </c>
       <c r="N38" s="283">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="O38" s="283">
         <f t="shared" si="1"/>
@@ -22640,7 +22727,7 @@
       </c>
       <c r="S38" s="285">
         <f>SUM(S7:S37)</f>
-        <v>18790</v>
+        <v>21913</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -24645,6 +24732,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -24661,12 +24754,6 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>